<commit_message>
Remove data sheet and added more problems
</commit_message>
<xml_diff>
--- a/0_Resources/Problems/2_Formulas_and_Functions_Problem.xlsx
+++ b/0_Resources/Problems/2_Formulas_and_Functions_Problem.xlsx
@@ -8,14 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SaderPC\Documents\GitHub\Excel_Data_Analytics_Course\0_Resources\Problems\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{605759A7-238D-43CC-9EAF-69A019D0CBC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8B84F4A-10BF-480E-B73B-C4C9664F7A4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{63EF8451-8C6D-4426-BE1B-F4EED8941AE0}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{63EF8451-8C6D-4426-BE1B-F4EED8941AE0}"/>
   </bookViews>
   <sheets>
-    <sheet name="Data" sheetId="2" r:id="rId1"/>
-    <sheet name="1_Formulas_Intro" sheetId="1" r:id="rId2"/>
-    <sheet name="2_Functions_Intro" sheetId="3" r:id="rId3"/>
+    <sheet name="1_Formulas_Intro" sheetId="1" r:id="rId1"/>
+    <sheet name="2_Functions_Intro" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="21">
   <si>
     <t>Job Title</t>
   </si>
@@ -82,13 +81,22 @@
     <t>2.1.6 - High Stock Options</t>
   </si>
   <si>
-    <t>2.2.3 Problem</t>
-  </si>
-  <si>
-    <t>2.1.7 Problem</t>
-  </si>
-  <si>
     <t>2.2.1 - Average Salary</t>
+  </si>
+  <si>
+    <t>2.1.3 - Total Compensation</t>
+  </si>
+  <si>
+    <t>2.1.10 - Problem</t>
+  </si>
+  <si>
+    <t>2.2.3 - Problem</t>
+  </si>
+  <si>
+    <t>2.2.5 - Problem</t>
+  </si>
+  <si>
+    <t>2.1.7 - Problem</t>
   </si>
 </sst>
 </file>
@@ -597,7 +605,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -608,6 +616,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="8" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="8" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -982,42 +991,64 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D81121F-E29F-4A0D-9A89-C1FE1C9EC139}">
-  <dimension ref="A1:H11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40322099-8982-4B34-B228-66F1BE7B0672}">
+  <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H11"/>
+      <selection activeCell="M1" sqref="I1:M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="9" max="9" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="33.140625" customWidth="1"/>
+    <col min="11" max="11" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1042,8 +1073,13 @@
       <c r="H2" s="3">
         <v>131.21</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2" s="8"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1068,8 +1104,13 @@
       <c r="H3" s="3">
         <v>168.6</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" s="8"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1094,8 +1135,13 @@
       <c r="H4" s="3">
         <v>257.32</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4" s="8"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1120,8 +1166,13 @@
       <c r="H5" s="3">
         <v>137.5</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5" s="8"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -1146,8 +1197,13 @@
       <c r="H6" s="3">
         <v>100.75</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6" s="8"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -1172,8 +1228,13 @@
       <c r="H7" s="3">
         <v>90.8</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7" s="8"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -1198,8 +1259,13 @@
       <c r="H8" s="3">
         <v>237.21</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8" s="8"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -1224,8 +1290,13 @@
       <c r="H9" s="3">
         <v>116.02</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9" s="8"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1250,8 +1321,13 @@
       <c r="H10" s="3">
         <v>200.01</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10" s="8"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -1276,6 +1352,11 @@
       <c r="H11" s="3">
         <v>274.58</v>
       </c>
+      <c r="I11" s="8"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1283,356 +1364,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40322099-8982-4B34-B228-66F1BE7B0672}">
-  <dimension ref="A1:K11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C165C161-A451-4687-91F4-38842B6C7924}">
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="9" max="9" width="33.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2">
-        <v>5</v>
-      </c>
-      <c r="C2" t="b">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1">
-        <v>134973</v>
-      </c>
-      <c r="E2" s="1">
-        <v>24000</v>
-      </c>
-      <c r="F2" s="2">
-        <v>0.05</v>
-      </c>
-      <c r="G2">
-        <v>41</v>
-      </c>
-      <c r="H2" s="3">
-        <v>131.21</v>
-      </c>
-      <c r="I2" s="8"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3">
-        <v>9</v>
-      </c>
-      <c r="C3" t="b">
-        <v>0</v>
-      </c>
-      <c r="D3" s="1">
-        <v>186476</v>
-      </c>
-      <c r="E3" s="1">
-        <v>17000</v>
-      </c>
-      <c r="F3" s="2">
-        <v>0.05</v>
-      </c>
-      <c r="G3">
-        <v>35</v>
-      </c>
-      <c r="H3" s="3">
-        <v>168.6</v>
-      </c>
-      <c r="I3" s="8"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4">
-        <v>5</v>
-      </c>
-      <c r="C4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D4" s="1">
-        <v>131845</v>
-      </c>
-      <c r="E4" s="1">
-        <v>9000</v>
-      </c>
-      <c r="F4" s="2">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="G4">
-        <v>44</v>
-      </c>
-      <c r="H4" s="3">
-        <v>257.32</v>
-      </c>
-      <c r="I4" s="8"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D5" s="1">
-        <v>181473</v>
-      </c>
-      <c r="E5" s="1">
-        <v>16000</v>
-      </c>
-      <c r="F5" s="2">
-        <v>0.04</v>
-      </c>
-      <c r="G5">
-        <v>21</v>
-      </c>
-      <c r="H5" s="3">
-        <v>137.5</v>
-      </c>
-      <c r="I5" s="8"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6">
-        <v>9</v>
-      </c>
-      <c r="C6" t="b">
-        <v>1</v>
-      </c>
-      <c r="D6" s="1">
-        <v>111262</v>
-      </c>
-      <c r="E6" s="1">
-        <v>19000</v>
-      </c>
-      <c r="F6" s="2">
-        <v>0.04</v>
-      </c>
-      <c r="G6">
-        <v>40</v>
-      </c>
-      <c r="H6" s="3">
-        <v>100.75</v>
-      </c>
-      <c r="I6" s="8"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7">
-        <v>4</v>
-      </c>
-      <c r="C7" t="b">
-        <v>1</v>
-      </c>
-      <c r="D7" s="1">
-        <v>117020</v>
-      </c>
-      <c r="E7" s="1">
-        <v>12000</v>
-      </c>
-      <c r="F7" s="2">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="G7">
-        <v>6</v>
-      </c>
-      <c r="H7" s="3">
-        <v>90.8</v>
-      </c>
-      <c r="I7" s="8"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="9"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8" t="b">
-        <v>0</v>
-      </c>
-      <c r="D8" s="1">
-        <v>126162</v>
-      </c>
-      <c r="E8" s="1">
-        <v>12000</v>
-      </c>
-      <c r="F8" s="2">
-        <v>5.5E-2</v>
-      </c>
-      <c r="G8">
-        <v>30</v>
-      </c>
-      <c r="H8" s="3">
-        <v>237.21</v>
-      </c>
-      <c r="I8" s="8"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9">
-        <v>7</v>
-      </c>
-      <c r="C9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D9" s="1">
-        <v>189073</v>
-      </c>
-      <c r="E9" s="1">
-        <v>17000</v>
-      </c>
-      <c r="F9" s="2">
-        <v>0.06</v>
-      </c>
-      <c r="G9">
-        <v>49</v>
-      </c>
-      <c r="H9" s="3">
-        <v>116.02</v>
-      </c>
-      <c r="I9" s="8"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <v>10</v>
-      </c>
-      <c r="C10" t="b">
-        <v>0</v>
-      </c>
-      <c r="D10" s="1">
-        <v>82495</v>
-      </c>
-      <c r="E10" s="1">
-        <v>26000</v>
-      </c>
-      <c r="F10" s="2">
-        <v>0.03</v>
-      </c>
-      <c r="G10">
-        <v>35</v>
-      </c>
-      <c r="H10" s="3">
-        <v>200.01</v>
-      </c>
-      <c r="I10" s="8"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11">
-        <v>5</v>
-      </c>
-      <c r="C11" t="b">
-        <v>1</v>
-      </c>
-      <c r="D11" s="1">
-        <v>134208</v>
-      </c>
-      <c r="E11" s="1">
-        <v>27000</v>
-      </c>
-      <c r="F11" s="2">
-        <v>5.5E-2</v>
-      </c>
-      <c r="G11">
-        <v>19</v>
-      </c>
-      <c r="H11" s="3">
-        <v>274.58</v>
-      </c>
-      <c r="I11" s="8"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C165C161-A451-4687-91F4-38842B6C7924}">
-  <dimension ref="A1:K11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1640,9 +1376,10 @@
     <col min="9" max="9" width="29.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1668,16 +1405,19 @@
         <v>7</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1705,8 +1445,9 @@
       <c r="I2" s="8"/>
       <c r="J2" s="9"/>
       <c r="K2" s="9"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2" s="9"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1734,7 +1475,7 @@
       <c r="I3" s="6"/>
       <c r="J3" s="9"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1762,7 +1503,7 @@
       <c r="I4" s="6"/>
       <c r="J4" s="9"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1790,7 +1531,7 @@
       <c r="I5" s="6"/>
       <c r="J5" s="9"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -1818,7 +1559,7 @@
       <c r="I6" s="6"/>
       <c r="J6" s="9"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -1846,7 +1587,7 @@
       <c r="I7" s="6"/>
       <c r="J7" s="9"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -1874,7 +1615,7 @@
       <c r="I8" s="6"/>
       <c r="J8" s="9"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -1902,7 +1643,7 @@
       <c r="I9" s="6"/>
       <c r="J9" s="9"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1930,7 +1671,7 @@
       <c r="I10" s="6"/>
       <c r="J10" s="9"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>

</xml_diff>